<commit_message>
planilha com dados é ida direitin
</commit_message>
<xml_diff>
--- a/Pórtico 1.xlsx
+++ b/Pórtico 1.xlsx
@@ -42,18 +42,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -283,16 +289,16 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.0</v>
       </c>
       <c r="D2" s="1">
@@ -304,7 +310,7 @@
       <c r="F2" s="1">
         <v>1.0</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="1">
@@ -316,16 +322,16 @@
       <c r="C3" s="1">
         <v>6.0</v>
       </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.0</v>
       </c>
       <c r="F3" s="1">
         <v>0.0</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="1">
@@ -346,7 +352,7 @@
       <c r="F4" s="1">
         <v>1.0</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1">
@@ -357,7 +363,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="1">
@@ -369,48 +375,48 @@
       <c r="C6" s="1">
         <v>2.0</v>
       </c>
-      <c r="D6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G6" s="2"/>
+      <c r="D6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="1">
         <v>2.0</v>
       </c>
-      <c r="B7" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="2">
         <v>3.0</v>
       </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="2"/>
+      <c r="D7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>2.0</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="1">
@@ -422,10 +428,12 @@
       <c r="C9" s="1">
         <v>0.0</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="1">
+        <v>0.0</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="1">
@@ -437,111 +445,113 @@
       <c r="C10" s="1">
         <v>-6.0</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1">
+        <v>0.0</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="1">
         <v>0.0</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>